<commit_message>
Update class reference docs
</commit_message>
<xml_diff>
--- a/notes/Request-response class reference.xlsx
+++ b/notes/Request-response class reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\IdeaProjects\jnano\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A2CC06-D47D-4B50-93C6-6FB195B7DD71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06428CBF-F548-4CE9-9D23-61DA7DADAEDD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{B9CF3A75-6AC5-46C2-8F87-C3B2BADF72E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="287">
   <si>
     <t>Command</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>Refer to command in node section</t>
+  </si>
+  <si>
+    <t>Use built in AccountAddress class for validation</t>
   </si>
 </sst>
 </file>
@@ -1322,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F51F2BD-F538-453A-AD22-77C6D703BF06}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,6 +2077,9 @@
       <c r="C65" s="10" t="s">
         <v>211</v>
       </c>
+      <c r="D65" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -2285,7 +2291,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -2392,7 +2398,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>60</v>
       </c>

</xml_diff>